<commit_message>
Update file name handling and summary new line handling.
</commit_message>
<xml_diff>
--- a/UseCaseTranslator/Resources/テストスイートテンプレート.xlsx
+++ b/UseCaseTranslator/Resources/テストスイートテンプレート.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\EAST\UseCaseTranslator\Solution\UseCaseTranslator\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\EAST\UseCaseTranslator\Solution.osada-jun\UseCaseTranslator\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="4875" windowWidth="28035" windowHeight="12555"/>
+    <workbookView xWindow="360" yWindow="9675" windowWidth="28035" windowHeight="12555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="概要" sheetId="9" r:id="rId1"/>
@@ -23,12 +23,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>長田 潤</author>
   </authors>
   <commentList>
-    <comment ref="C6" authorId="0" shapeId="0">
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
@@ -954,10 +954,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1006,12 +1006,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.35"/>
@@ -1080,7 +1080,7 @@
       <c r="H5" s="20"/>
       <c r="I5" s="21"/>
     </row>
-    <row r="6" spans="1:9" ht="24" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="117.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="31" t="s">
         <v>18</v>
       </c>
@@ -1889,7 +1889,10 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="12" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;P ページ</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>